<commit_message>
Xin modified for submittion
</commit_message>
<xml_diff>
--- a/Results/EMRSpark.xlsx
+++ b/Results/EMRSpark.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xin Yang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yx960203/Desktop/Code/559/project_cc/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12350"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>WORDCOUNT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,38 +128,66 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>infinite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>StandardDeviationOfRecords</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Air Quality</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Round</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>SumofRecords</t>
+  </si>
+  <si>
+    <t>Air Quality</t>
+  </si>
+  <si>
+    <t>Hash Algorithms</t>
+  </si>
+  <si>
+    <t>Time/s</t>
+  </si>
+  <si>
+    <t>Distribution Conditions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -176,21 +210,75 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,18 +558,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.25" customWidth="1"/>
-    <col min="23" max="23" width="8.6640625" style="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="23" max="23" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,17 +580,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="G2" t="s">
         <v>16</v>
       </c>
       <c r="X2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -510,6 +598,9 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
       <c r="G3">
         <v>1</v>
       </c>
@@ -589,17 +680,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <f>AVERAGE(X5:AG5)</f>
+        <f t="shared" ref="C5:C18" si="0">AVERAGE(X5:AG5)</f>
         <v>28.4</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E17" si="0">STDEV(G5:V5)</f>
+        <f t="shared" ref="E5:E17" si="1">STDEV(G5:V5)</f>
         <v>6.1478315960453349</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F18" si="2">SUM(G5:V5)</f>
+        <v>559</v>
       </c>
       <c r="G5" s="1">
         <v>33</v>
@@ -680,53 +775,57 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <f>AVERAGE(X6:AG6)</f>
         <v>28</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>3.0214510862608162</v>
+        <f>STDEV(G6:V6)</f>
+        <v>5.2974050251042728</v>
+      </c>
+      <c r="F6" s="1">
+        <f>SUM(G6:V6)</f>
+        <v>559</v>
       </c>
       <c r="G6" s="1">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H6">
+        <v>27</v>
+      </c>
+      <c r="I6">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>35</v>
+      </c>
+      <c r="K6">
+        <v>45</v>
+      </c>
+      <c r="L6">
+        <v>28</v>
+      </c>
+      <c r="M6">
         <v>37</v>
-      </c>
-      <c r="I6">
-        <v>35</v>
-      </c>
-      <c r="J6">
-        <v>32</v>
-      </c>
-      <c r="K6">
-        <v>30</v>
-      </c>
-      <c r="L6">
-        <v>31</v>
-      </c>
-      <c r="M6">
-        <v>32</v>
       </c>
       <c r="N6">
         <v>35</v>
       </c>
       <c r="O6">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="P6">
         <v>36</v>
       </c>
       <c r="Q6">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="R6">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="S6">
         <v>36</v>
@@ -735,43 +834,43 @@
         <v>36</v>
       </c>
       <c r="U6">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="V6">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="X6" s="1">
+        <v>27</v>
+      </c>
+      <c r="Y6" s="1">
         <v>28</v>
       </c>
-      <c r="Y6" s="1">
-        <v>27</v>
-      </c>
       <c r="Z6" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AA6" s="1">
         <v>28</v>
       </c>
       <c r="AB6" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AC6" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AD6" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AE6" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AF6" s="1">
         <v>29</v>
       </c>
       <c r="AG6" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -780,8 +879,12 @@
         <v>28.5</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f>STDEV(G7:V7)</f>
         <v>6.0494490107226566</v>
+      </c>
+      <c r="F7" s="1">
+        <f>SUM(G7:V7)</f>
+        <v>559</v>
       </c>
       <c r="G7" s="1">
         <v>31</v>
@@ -862,53 +965,57 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
-        <f>AVERAGE(X8:AG8)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>5.2974050251042728</v>
+        <f t="shared" si="1"/>
+        <v>3.0214510862608162</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
       </c>
       <c r="G8" s="1">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="I8">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J8">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K8">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="L8">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M8">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="N8">
         <v>35</v>
       </c>
       <c r="O8">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="P8">
         <v>36</v>
       </c>
       <c r="Q8">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R8">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="S8">
         <v>36</v>
@@ -917,53 +1024,57 @@
         <v>36</v>
       </c>
       <c r="U8">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="V8">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="X8" s="1">
+        <v>28</v>
+      </c>
+      <c r="Y8" s="1">
         <v>27</v>
       </c>
-      <c r="Y8" s="1">
-        <v>28</v>
-      </c>
       <c r="Z8" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AA8" s="1">
         <v>28</v>
       </c>
       <c r="AB8" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AC8" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AD8" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AE8" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AF8" s="1">
         <v>29</v>
       </c>
       <c r="AG8" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <f>AVERAGE(X9:AG9)</f>
+        <f t="shared" si="0"/>
         <v>35.200000000000003</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5163256517764667</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
       </c>
       <c r="G9" s="1">
         <v>34</v>
@@ -1044,17 +1155,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1">
-        <f>AVERAGE(X10:AG10)</f>
+        <f t="shared" si="0"/>
         <v>29.7</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.72774107706294</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
       </c>
       <c r="G10" s="1">
         <v>43</v>
@@ -1135,156 +1250,164 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
         <f>AVERAGE(X11:AG11)</f>
-        <v>28.5</v>
+        <v>29.6</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>4.0409363601356887</v>
+        <f>STDEV(G11:V11)</f>
+        <v>31.716386406188626</v>
+      </c>
+      <c r="F11" s="1">
+        <f>SUM(G11:V11)</f>
+        <v>559</v>
       </c>
       <c r="G11" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H11">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="I11">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="K11">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="L11">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="M11">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="N11">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="O11">
         <v>35</v>
       </c>
       <c r="P11">
+        <v>39</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>30</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>29</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>30</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>29</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>30</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>30</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>29</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>31</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>29</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>28.5</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0409363601356887</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
+      </c>
+      <c r="G12" s="1">
+        <v>39</v>
+      </c>
+      <c r="H12">
+        <v>36</v>
+      </c>
+      <c r="I12">
+        <v>35</v>
+      </c>
+      <c r="J12">
+        <v>31</v>
+      </c>
+      <c r="K12">
+        <v>35</v>
+      </c>
+      <c r="L12">
+        <v>35</v>
+      </c>
+      <c r="M12">
         <v>32</v>
       </c>
-      <c r="Q11">
-        <v>33</v>
-      </c>
-      <c r="R11">
-        <v>40</v>
-      </c>
-      <c r="S11">
-        <v>36</v>
-      </c>
-      <c r="T11">
-        <v>44</v>
-      </c>
-      <c r="U11">
-        <v>36</v>
-      </c>
-      <c r="V11">
-        <v>34</v>
-      </c>
-      <c r="X11" s="1">
-        <v>30</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>29</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>27</v>
-      </c>
-      <c r="AA11" s="1">
-        <v>28</v>
-      </c>
-      <c r="AB11" s="1">
-        <v>28</v>
-      </c>
-      <c r="AC11" s="1">
-        <v>29</v>
-      </c>
-      <c r="AD11" s="1">
-        <v>28</v>
-      </c>
-      <c r="AE11" s="1">
-        <v>32</v>
-      </c>
-      <c r="AF11" s="1">
-        <v>27</v>
-      </c>
-      <c r="AG11" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1">
-        <f>AVERAGE(X12:AG12)</f>
-        <v>29.6</v>
-      </c>
-      <c r="E12" s="1">
-        <f>STDEV(G12:V12)</f>
-        <v>31.716386406188626</v>
-      </c>
-      <c r="G12" s="1">
-        <v>37</v>
-      </c>
-      <c r="H12">
-        <v>65</v>
-      </c>
-      <c r="I12">
-        <v>88</v>
-      </c>
-      <c r="J12">
-        <v>71</v>
-      </c>
-      <c r="K12">
-        <v>53</v>
-      </c>
-      <c r="L12">
-        <v>77</v>
-      </c>
-      <c r="M12">
-        <v>60</v>
-      </c>
       <c r="N12">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="O12">
         <v>35</v>
       </c>
       <c r="P12">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="X12" s="1">
         <v>30</v>
@@ -1293,92 +1416,96 @@
         <v>29</v>
       </c>
       <c r="Z12" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AA12" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB12" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AC12" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AD12" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AE12" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AF12" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AG12" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
         <f>AVERAGE(X13:AG13)</f>
-        <v>28.6</v>
+        <v>28.8</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>8.7442838471769662</v>
+        <f>STDEV(G13:V13)</f>
+        <v>2.8860295678781025</v>
+      </c>
+      <c r="F13" s="1">
+        <f>SUM(G13:V13)</f>
+        <v>559</v>
       </c>
       <c r="G13" s="1">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H13">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I13">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J13">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="L13">
         <v>38</v>
       </c>
       <c r="M13">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="N13">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="O13">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="P13">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="Q13">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="R13">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="S13">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="T13">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="U13">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="V13">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="X13" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Y13" s="1">
         <v>30</v>
@@ -1387,89 +1514,93 @@
         <v>27</v>
       </c>
       <c r="AA13" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB13" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC13" s="1">
+        <v>30</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>30</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>27</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>27</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>28.6</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>8.7442838471769662</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
+      </c>
+      <c r="G14" s="1">
+        <v>23</v>
+      </c>
+      <c r="H14">
         <v>28</v>
       </c>
-      <c r="AD13" s="1">
-        <v>28</v>
-      </c>
-      <c r="AE13" s="1">
-        <v>31</v>
-      </c>
-      <c r="AF13" s="1">
-        <v>29</v>
-      </c>
-      <c r="AG13" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1">
-        <f>AVERAGE(X14:AG14)</f>
-        <v>28.8</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>2.8860295678781025</v>
-      </c>
-      <c r="G14" s="1">
-        <v>35</v>
-      </c>
-      <c r="H14">
-        <v>35</v>
-      </c>
       <c r="I14">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J14">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K14">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="L14">
         <v>38</v>
       </c>
       <c r="M14">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="N14">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="O14">
+        <v>46</v>
+      </c>
+      <c r="P14">
+        <v>45</v>
+      </c>
+      <c r="Q14">
+        <v>41</v>
+      </c>
+      <c r="R14">
         <v>36</v>
       </c>
-      <c r="P14">
-        <v>36</v>
-      </c>
-      <c r="Q14">
-        <v>28</v>
-      </c>
-      <c r="R14">
-        <v>38</v>
-      </c>
       <c r="S14">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="T14">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="U14">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="V14">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="X14" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Y14" s="1">
         <v>30</v>
@@ -1478,38 +1609,42 @@
         <v>27</v>
       </c>
       <c r="AA14" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AB14" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC14" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AD14" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AE14" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="AF14" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AG14" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="C15">
-        <f>AVERAGE(X15:AG15)</f>
+        <f t="shared" si="0"/>
         <v>27.9</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.7442838471769662</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
       </c>
       <c r="G15" s="1">
         <v>23</v>
@@ -1590,17 +1725,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1">
-        <f>AVERAGE(X16:AG16)</f>
+        <f t="shared" si="0"/>
         <v>28.4</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3889064697256881</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
       </c>
       <c r="G16" s="1">
         <v>36</v>
@@ -1681,17 +1820,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1">
-        <f>AVERAGE(X17:AG17)</f>
+        <f t="shared" si="0"/>
         <v>29.5</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>67.056661364351669</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
       </c>
       <c r="G17" s="1">
         <v>277</v>
@@ -1772,17 +1915,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="1">
-        <f>AVERAGE(X18:AG18)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E18" si="1">STDEV(G18:V18)</f>
+        <f t="shared" ref="E18" si="3">STDEV(G18:V18)</f>
         <v>139.75</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>559</v>
       </c>
       <c r="G18" s="1">
         <v>559</v>
@@ -1863,7 +2010,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1872,18 +2019,18 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="1">
-        <f>AVERAGE(X22:AG22)</f>
+        <f t="shared" ref="C22:C25" si="4">AVERAGE(X22:AG22)</f>
         <v>44.9</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="2">
         <f>STDEV(G22:V22)</f>
         <v>538.31490164524826</v>
       </c>
@@ -1966,107 +2113,107 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1">
-        <f>AVERAGE(X23:AG23)</f>
-        <v>43.5</v>
-      </c>
-      <c r="E23" s="1">
-        <f>STDEV(G23:V23)</f>
-        <v>671.20965428098543</v>
+        <f t="shared" si="4"/>
+        <v>46.8</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" ref="E23:E33" si="5">STDEV(G23:V23)</f>
+        <v>559.58425043359944</v>
       </c>
       <c r="G23">
-        <v>55170</v>
+        <v>54754</v>
       </c>
       <c r="H23">
-        <v>55429</v>
+        <v>54499</v>
       </c>
       <c r="I23">
-        <v>54163</v>
+        <v>54229</v>
       </c>
       <c r="J23">
-        <v>54654</v>
+        <v>54113</v>
       </c>
       <c r="K23">
-        <v>53563</v>
+        <v>54824</v>
       </c>
       <c r="L23">
-        <v>54099</v>
+        <v>54948</v>
       </c>
       <c r="M23">
-        <v>54540</v>
+        <v>54349</v>
       </c>
       <c r="N23">
-        <v>54004</v>
+        <v>55101</v>
       </c>
       <c r="O23">
-        <v>53686</v>
+        <v>55341</v>
       </c>
       <c r="P23">
-        <v>56072</v>
+        <v>53362</v>
       </c>
       <c r="Q23">
-        <v>54291</v>
+        <v>54718</v>
       </c>
       <c r="R23">
-        <v>54239</v>
+        <v>53709</v>
       </c>
       <c r="S23">
-        <v>55035</v>
+        <v>55000</v>
       </c>
       <c r="T23">
-        <v>54541</v>
+        <v>54615</v>
       </c>
       <c r="U23">
-        <v>53804</v>
+        <v>53613</v>
       </c>
       <c r="V23">
-        <v>54398</v>
-      </c>
-      <c r="X23" s="1">
+        <v>54513</v>
+      </c>
+      <c r="X23">
+        <v>46</v>
+      </c>
+      <c r="Y23">
+        <v>66</v>
+      </c>
+      <c r="Z23">
+        <v>44</v>
+      </c>
+      <c r="AA23">
         <v>43</v>
       </c>
-      <c r="Y23" s="1">
+      <c r="AB23">
         <v>45</v>
       </c>
-      <c r="Z23" s="1">
+      <c r="AC23">
         <v>44</v>
       </c>
-      <c r="AA23" s="1">
-        <v>42</v>
-      </c>
-      <c r="AB23" s="1">
+      <c r="AD23">
+        <v>44</v>
+      </c>
+      <c r="AE23">
         <v>45</v>
       </c>
-      <c r="AC23" s="1">
+      <c r="AF23">
+        <v>47</v>
+      </c>
+      <c r="AG23">
         <v>44</v>
       </c>
-      <c r="AD23" s="1">
-        <v>42</v>
-      </c>
-      <c r="AE23" s="1">
-        <v>43</v>
-      </c>
-      <c r="AF23" s="1">
-        <v>43</v>
-      </c>
-      <c r="AG23" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="1">
-        <f>AVERAGE(X24:AG24)</f>
+        <f t="shared" si="4"/>
         <v>43.9</v>
       </c>
-      <c r="E24" s="1">
-        <f>STDEV(G24:V24)</f>
+      <c r="E24" s="2">
+        <f t="shared" si="5"/>
         <v>456.01388867738081</v>
       </c>
       <c r="G24">
@@ -2148,114 +2295,118 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1">
-        <f>AVERAGE(X25:AG25)</f>
-        <v>46.8</v>
-      </c>
-      <c r="E25" s="1">
-        <f>STDEV(G25:V25)</f>
-        <v>559.58425043359944</v>
+        <f t="shared" si="4"/>
+        <v>43.5</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="5"/>
+        <v>671.20965428098543</v>
       </c>
       <c r="G25">
-        <v>54754</v>
+        <v>55170</v>
       </c>
       <c r="H25">
-        <v>54499</v>
+        <v>55429</v>
       </c>
       <c r="I25">
-        <v>54229</v>
+        <v>54163</v>
       </c>
       <c r="J25">
-        <v>54113</v>
+        <v>54654</v>
       </c>
       <c r="K25">
-        <v>54824</v>
+        <v>53563</v>
       </c>
       <c r="L25">
-        <v>54948</v>
+        <v>54099</v>
       </c>
       <c r="M25">
-        <v>54349</v>
+        <v>54540</v>
       </c>
       <c r="N25">
-        <v>55101</v>
+        <v>54004</v>
       </c>
       <c r="O25">
-        <v>55341</v>
+        <v>53686</v>
       </c>
       <c r="P25">
-        <v>53362</v>
+        <v>56072</v>
       </c>
       <c r="Q25">
-        <v>54718</v>
+        <v>54291</v>
       </c>
       <c r="R25">
-        <v>53709</v>
+        <v>54239</v>
       </c>
       <c r="S25">
-        <v>55000</v>
+        <v>55035</v>
       </c>
       <c r="T25">
-        <v>54615</v>
+        <v>54541</v>
       </c>
       <c r="U25">
-        <v>53613</v>
+        <v>53804</v>
       </c>
       <c r="V25">
-        <v>54513</v>
-      </c>
-      <c r="X25">
-        <v>46</v>
-      </c>
-      <c r="Y25">
-        <v>66</v>
-      </c>
-      <c r="Z25">
+        <v>54398</v>
+      </c>
+      <c r="X25" s="1">
+        <v>43</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>45</v>
+      </c>
+      <c r="Z25" s="1">
         <v>44</v>
       </c>
-      <c r="AA25">
+      <c r="AA25" s="1">
+        <v>42</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>45</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>44</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>42</v>
+      </c>
+      <c r="AE25" s="1">
         <v>43</v>
       </c>
-      <c r="AB25">
-        <v>45</v>
-      </c>
-      <c r="AC25">
+      <c r="AF25" s="1">
+        <v>43</v>
+      </c>
+      <c r="AG25" s="1">
         <v>44</v>
       </c>
-      <c r="AD25">
-        <v>44</v>
-      </c>
-      <c r="AE25">
-        <v>45</v>
-      </c>
-      <c r="AF25">
-        <v>47</v>
-      </c>
-      <c r="AG25">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="1">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="1">
-        <v>200</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" ref="E27:E34" si="2">STDEV(G27:V27)</f>
+      <c r="C27">
+        <f>AVERAGE(X27:AG27)</f>
+        <v>128.4</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="5"/>
         <v>467.79069393622331</v>
       </c>
       <c r="G27">
@@ -2337,198 +2488,198 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" ref="C28:C34" si="6">AVERAGE(X28:AG28)</f>
+        <v>118.8</v>
+      </c>
+      <c r="E28" s="1">
+        <f>STDEV(G28:V28)</f>
+        <v>48672.497138870254</v>
+      </c>
+      <c r="G28">
+        <v>55569</v>
+      </c>
+      <c r="H28">
+        <v>109632</v>
+      </c>
+      <c r="I28">
+        <v>108614</v>
+      </c>
+      <c r="J28">
+        <v>108396</v>
+      </c>
+      <c r="K28">
+        <v>108863</v>
+      </c>
+      <c r="L28">
+        <v>107123</v>
+      </c>
+      <c r="M28">
+        <v>110309</v>
+      </c>
+      <c r="N28">
+        <v>53853</v>
+      </c>
+      <c r="O28">
+        <v>55031</v>
+      </c>
+      <c r="P28">
+        <v>54298</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>120</v>
+      </c>
+      <c r="Y28">
+        <v>120</v>
+      </c>
+      <c r="Z28">
+        <v>120</v>
+      </c>
+      <c r="AA28">
+        <v>120</v>
+      </c>
+      <c r="AB28">
+        <v>120</v>
+      </c>
+      <c r="AC28">
+        <v>120</v>
+      </c>
+      <c r="AD28">
+        <v>120</v>
+      </c>
+      <c r="AE28">
+        <v>114</v>
+      </c>
+      <c r="AF28">
+        <v>120</v>
+      </c>
+      <c r="AG28">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="1">
-        <f>AVERAGE(X28:AG28)</f>
+      <c r="C29" s="1">
+        <f t="shared" si="6"/>
         <v>60.5</v>
       </c>
-      <c r="E28" s="1">
-        <f t="shared" si="2"/>
+      <c r="E29" s="2">
+        <f t="shared" si="5"/>
         <v>579.20267034375229</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>55905</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>54086</v>
       </c>
-      <c r="I28">
+      <c r="I29">
         <v>53870</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>54509</v>
       </c>
-      <c r="K28">
+      <c r="K29">
         <v>54418</v>
       </c>
-      <c r="L28">
+      <c r="L29">
         <v>54732</v>
       </c>
-      <c r="M28">
+      <c r="M29">
         <v>54593</v>
       </c>
-      <c r="N28">
+      <c r="N29">
         <v>54244</v>
       </c>
-      <c r="O28">
+      <c r="O29">
         <v>54941</v>
       </c>
-      <c r="P28">
+      <c r="P29">
         <v>53589</v>
       </c>
-      <c r="Q28">
+      <c r="Q29">
         <v>55355</v>
       </c>
-      <c r="R28">
+      <c r="R29">
         <v>54442</v>
       </c>
-      <c r="S28">
+      <c r="S29">
         <v>53960</v>
       </c>
-      <c r="T28">
+      <c r="T29">
         <v>54157</v>
       </c>
-      <c r="U28">
+      <c r="U29">
         <v>54138</v>
       </c>
-      <c r="V28">
+      <c r="V29">
         <v>54749</v>
       </c>
-      <c r="X28" s="1">
+      <c r="X29" s="1">
         <v>57</v>
       </c>
-      <c r="Y28" s="1">
+      <c r="Y29" s="1">
         <v>59</v>
       </c>
-      <c r="Z28" s="1">
+      <c r="Z29" s="1">
         <v>60</v>
       </c>
-      <c r="AA28" s="1">
+      <c r="AA29" s="1">
         <v>72</v>
       </c>
-      <c r="AB28" s="1">
+      <c r="AB29" s="1">
         <v>59</v>
       </c>
-      <c r="AC28" s="1">
+      <c r="AC29" s="1">
         <v>66</v>
       </c>
-      <c r="AD28" s="1">
+      <c r="AD29" s="1">
         <v>58</v>
       </c>
-      <c r="AE28" s="1">
+      <c r="AE29" s="1">
         <v>59</v>
       </c>
-      <c r="AF28" s="1">
+      <c r="AF29" s="1">
         <v>59</v>
       </c>
-      <c r="AG28" s="1">
+      <c r="AG29" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1">
-        <f>AVERAGE(X29:AG29)</f>
-        <v>47.8</v>
-      </c>
-      <c r="E29" s="1">
-        <f>STDEV(G29:V29)</f>
-        <v>3365.8698374268724</v>
-      </c>
-      <c r="G29">
-        <v>78365</v>
-      </c>
-      <c r="H29">
-        <v>78918</v>
-      </c>
-      <c r="I29">
-        <v>69991</v>
-      </c>
-      <c r="J29">
-        <v>73970</v>
-      </c>
-      <c r="K29">
-        <v>72213</v>
-      </c>
-      <c r="L29">
-        <v>69839</v>
-      </c>
-      <c r="M29">
-        <v>68118</v>
-      </c>
-      <c r="N29">
-        <v>72088</v>
-      </c>
-      <c r="O29">
-        <v>72070</v>
-      </c>
-      <c r="P29">
-        <v>70368</v>
-      </c>
-      <c r="Q29">
-        <v>67828</v>
-      </c>
-      <c r="R29">
-        <v>69433</v>
-      </c>
-      <c r="S29">
-        <v>71212</v>
-      </c>
-      <c r="T29">
-        <v>68635</v>
-      </c>
-      <c r="U29">
-        <v>69111</v>
-      </c>
-      <c r="V29">
-        <v>68052</v>
-      </c>
-      <c r="X29" s="1">
-        <v>46</v>
-      </c>
-      <c r="Y29" s="1">
-        <v>45</v>
-      </c>
-      <c r="Z29" s="1">
-        <v>52</v>
-      </c>
-      <c r="AA29" s="1">
-        <v>48</v>
-      </c>
-      <c r="AB29" s="1">
-        <v>46</v>
-      </c>
-      <c r="AC29" s="1">
-        <v>47</v>
-      </c>
-      <c r="AD29" s="1">
-        <v>57</v>
-      </c>
-      <c r="AE29" s="1">
-        <v>44</v>
-      </c>
-      <c r="AF29" s="1">
-        <v>46</v>
-      </c>
-      <c r="AG29" s="1">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="1">
-        <f>AVERAGE(X30:AG30)</f>
+        <f t="shared" si="6"/>
         <v>52.6</v>
       </c>
-      <c r="E30">
-        <f t="shared" si="2"/>
+      <c r="E30" s="2">
+        <f t="shared" si="5"/>
         <v>535.18694553087391</v>
       </c>
       <c r="G30">
@@ -2610,385 +2761,387 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <f>AVERAGE(X31:AG31)</f>
-        <v>46.3</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" si="2"/>
-        <v>738.94724383183586</v>
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="6"/>
+        <v>47.8</v>
+      </c>
+      <c r="E31" s="2">
+        <f>STDEV(G31:V31)</f>
+        <v>3365.8698374268724</v>
       </c>
       <c r="G31">
-        <v>54794</v>
+        <v>78365</v>
       </c>
       <c r="H31">
-        <v>56688</v>
+        <v>78918</v>
       </c>
       <c r="I31">
-        <v>56320</v>
+        <v>69991</v>
       </c>
       <c r="J31">
-        <v>55758</v>
+        <v>73970</v>
       </c>
       <c r="K31">
-        <v>54420</v>
+        <v>72213</v>
       </c>
       <c r="L31">
-        <v>56080</v>
+        <v>69839</v>
       </c>
       <c r="M31">
-        <v>54921</v>
+        <v>68118</v>
       </c>
       <c r="N31">
-        <v>55589</v>
+        <v>72088</v>
       </c>
       <c r="O31">
-        <v>55923</v>
+        <v>72070</v>
       </c>
       <c r="P31">
-        <v>56455</v>
+        <v>70368</v>
       </c>
       <c r="Q31">
-        <v>55517</v>
+        <v>67828</v>
       </c>
       <c r="R31">
-        <v>55856</v>
+        <v>69433</v>
       </c>
       <c r="S31">
-        <v>55448</v>
+        <v>71212</v>
       </c>
       <c r="T31">
-        <v>55108</v>
+        <v>68635</v>
       </c>
       <c r="U31">
-        <v>54289</v>
+        <v>69111</v>
       </c>
       <c r="V31">
-        <v>54573</v>
+        <v>68052</v>
       </c>
       <c r="X31" s="1">
+        <v>46</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>45</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>52</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>48</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>46</v>
+      </c>
+      <c r="AC31" s="1">
         <v>47</v>
       </c>
-      <c r="Y31" s="1">
-        <v>46</v>
-      </c>
-      <c r="Z31" s="1">
-        <v>47</v>
-      </c>
-      <c r="AA31" s="1">
-        <v>50</v>
-      </c>
-      <c r="AB31" s="1">
-        <v>49</v>
-      </c>
-      <c r="AC31" s="1">
-        <v>46</v>
-      </c>
       <c r="AD31" s="1">
+        <v>57</v>
+      </c>
+      <c r="AE31" s="1">
         <v>44</v>
-      </c>
-      <c r="AE31" s="1">
-        <v>45</v>
       </c>
       <c r="AF31" s="1">
         <v>46</v>
       </c>
       <c r="AG31" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="6"/>
+        <v>46.3</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="5"/>
+        <v>738.94724383183586</v>
+      </c>
+      <c r="G32">
+        <v>54794</v>
+      </c>
+      <c r="H32">
+        <v>56688</v>
+      </c>
+      <c r="I32">
+        <v>56320</v>
+      </c>
+      <c r="J32">
+        <v>55758</v>
+      </c>
+      <c r="K32">
+        <v>54420</v>
+      </c>
+      <c r="L32">
+        <v>56080</v>
+      </c>
+      <c r="M32">
+        <v>54921</v>
+      </c>
+      <c r="N32">
+        <v>55589</v>
+      </c>
+      <c r="O32">
+        <v>55923</v>
+      </c>
+      <c r="P32">
+        <v>56455</v>
+      </c>
+      <c r="Q32">
+        <v>55517</v>
+      </c>
+      <c r="R32">
+        <v>55856</v>
+      </c>
+      <c r="S32">
+        <v>55448</v>
+      </c>
+      <c r="T32">
+        <v>55108</v>
+      </c>
+      <c r="U32">
+        <v>54289</v>
+      </c>
+      <c r="V32">
+        <v>54573</v>
+      </c>
+      <c r="X32" s="1">
+        <v>47</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>46</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>47</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>50</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>49</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>46</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>44</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>45</v>
+      </c>
+      <c r="AF32" s="1">
+        <v>46</v>
+      </c>
+      <c r="AG32" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="1">
-        <f>AVERAGE(X32:AG32)</f>
+      <c r="C33" s="1">
+        <f t="shared" si="6"/>
         <v>88.8</v>
       </c>
-      <c r="E32" s="1">
-        <f t="shared" si="2"/>
+      <c r="E33" s="2">
+        <f t="shared" si="5"/>
         <v>528.43113710933676</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>54638</v>
       </c>
-      <c r="H32">
+      <c r="H33">
         <v>53866</v>
       </c>
-      <c r="I32">
+      <c r="I33">
         <v>54119</v>
       </c>
-      <c r="J32">
+      <c r="J33">
         <v>54046</v>
       </c>
-      <c r="K32">
+      <c r="K33">
         <v>54543</v>
       </c>
-      <c r="L32">
+      <c r="L33">
         <v>53838</v>
       </c>
-      <c r="M32">
+      <c r="M33">
         <v>54021</v>
       </c>
-      <c r="N32">
+      <c r="N33">
         <v>53877</v>
       </c>
-      <c r="O32">
+      <c r="O33">
         <v>55275</v>
       </c>
-      <c r="P32">
+      <c r="P33">
         <v>55140</v>
       </c>
-      <c r="Q32">
+      <c r="Q33">
         <v>55217</v>
       </c>
-      <c r="R32">
+      <c r="R33">
         <v>54475</v>
       </c>
-      <c r="S32">
+      <c r="S33">
         <v>55068</v>
       </c>
-      <c r="T32">
+      <c r="T33">
         <v>53998</v>
       </c>
-      <c r="U32">
+      <c r="U33">
         <v>54555</v>
       </c>
-      <c r="V32">
+      <c r="V33">
         <v>55012</v>
       </c>
-      <c r="X32">
+      <c r="X33">
         <v>90</v>
       </c>
-      <c r="Y32">
+      <c r="Y33">
         <v>96</v>
       </c>
-      <c r="Z32">
+      <c r="Z33">
         <v>78</v>
       </c>
-      <c r="AA32">
+      <c r="AA33">
         <v>90</v>
       </c>
-      <c r="AB32">
+      <c r="AB33">
         <v>96</v>
       </c>
-      <c r="AC32">
+      <c r="AC33">
         <v>90</v>
-      </c>
-      <c r="AD32">
-        <v>90</v>
-      </c>
-      <c r="AE32">
-        <v>96</v>
-      </c>
-      <c r="AF32">
-        <v>78</v>
-      </c>
-      <c r="AG32">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="1">
-        <f>AVERAGE(X33:AG33)</f>
-        <v>87</v>
-      </c>
-      <c r="E33" s="1">
-        <f>STDEV(G33:V33)</f>
-        <v>55808.625864944333</v>
-      </c>
-      <c r="G33">
-        <v>243878</v>
-      </c>
-      <c r="H33">
-        <v>64454</v>
-      </c>
-      <c r="I33">
-        <v>62344</v>
-      </c>
-      <c r="J33">
-        <v>33663</v>
-      </c>
-      <c r="K33">
-        <v>91852</v>
-      </c>
-      <c r="L33">
-        <v>49062</v>
-      </c>
-      <c r="M33">
-        <v>40158</v>
-      </c>
-      <c r="N33">
-        <v>39293</v>
-      </c>
-      <c r="O33">
-        <v>82292</v>
-      </c>
-      <c r="P33">
-        <v>17899</v>
-      </c>
-      <c r="Q33">
-        <v>27531</v>
-      </c>
-      <c r="R33">
-        <v>8886</v>
-      </c>
-      <c r="S33">
-        <v>47703</v>
-      </c>
-      <c r="T33">
-        <v>17949</v>
-      </c>
-      <c r="U33">
-        <v>26278</v>
-      </c>
-      <c r="V33">
-        <v>18446</v>
-      </c>
-      <c r="X33">
-        <v>84</v>
-      </c>
-      <c r="Y33">
-        <v>84</v>
-      </c>
-      <c r="Z33">
-        <v>84</v>
-      </c>
-      <c r="AA33">
-        <v>96</v>
-      </c>
-      <c r="AB33">
-        <v>84</v>
-      </c>
-      <c r="AC33">
-        <v>84</v>
       </c>
       <c r="AD33">
         <v>90</v>
       </c>
       <c r="AE33">
+        <v>96</v>
+      </c>
+      <c r="AF33">
+        <v>78</v>
+      </c>
+      <c r="AG33">
         <v>84</v>
       </c>
-      <c r="AF33">
-        <v>90</v>
-      </c>
-      <c r="AG33">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1">
-        <f>AVERAGE(X34:AG34)</f>
-        <v>118.8</v>
+        <f t="shared" si="6"/>
+        <v>87</v>
       </c>
       <c r="E34" s="1">
         <f>STDEV(G34:V34)</f>
-        <v>48672.497138870254</v>
+        <v>55808.625864944333</v>
       </c>
       <c r="G34">
-        <v>55569</v>
+        <v>243878</v>
       </c>
       <c r="H34">
-        <v>109632</v>
+        <v>64454</v>
       </c>
       <c r="I34">
-        <v>108614</v>
+        <v>62344</v>
       </c>
       <c r="J34">
-        <v>108396</v>
+        <v>33663</v>
       </c>
       <c r="K34">
-        <v>108863</v>
+        <v>91852</v>
       </c>
       <c r="L34">
-        <v>107123</v>
+        <v>49062</v>
       </c>
       <c r="M34">
-        <v>110309</v>
+        <v>40158</v>
       </c>
       <c r="N34">
-        <v>53853</v>
+        <v>39293</v>
       </c>
       <c r="O34">
-        <v>55031</v>
+        <v>82292</v>
       </c>
       <c r="P34">
-        <v>54298</v>
+        <v>17899</v>
       </c>
       <c r="Q34">
-        <v>0</v>
+        <v>27531</v>
       </c>
       <c r="R34">
-        <v>0</v>
+        <v>8886</v>
       </c>
       <c r="S34">
-        <v>0</v>
+        <v>47703</v>
       </c>
       <c r="T34">
-        <v>0</v>
+        <v>17949</v>
       </c>
       <c r="U34">
-        <v>0</v>
+        <v>26278</v>
       </c>
       <c r="V34">
-        <v>0</v>
+        <v>18446</v>
       </c>
       <c r="X34">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="Y34">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="Z34">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="AA34">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="AB34">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="AC34">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="AD34">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="AE34">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="AF34">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="AG34">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="1">
-        <v>200</v>
-      </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="E37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -2998,18 +3151,25 @@
       <c r="E39" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="F39" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="1">
-        <f>AVERAGE(X41:AG41)</f>
+        <f t="shared" ref="C41:C54" si="7">AVERAGE(X41:AG41)</f>
         <v>30.2</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" ref="E41:E48" si="3">STDEV(G41:V41)</f>
+        <f t="shared" ref="E41:E48" si="8">STDEV(G41:V41)</f>
         <v>17.921588471263739</v>
+      </c>
+      <c r="F41">
+        <f>SUM(G41:V41)</f>
+        <v>1410</v>
       </c>
       <c r="G41">
         <v>83</v>
@@ -3090,98 +3250,102 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C42" s="1">
         <f>AVERAGE(X42:AG42)</f>
-        <v>29.9</v>
+        <v>29</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="3"/>
-        <v>11.988188631593459</v>
+        <f>STDEV(G42:V42)</f>
+        <v>16.839932699786342</v>
+      </c>
+      <c r="F42" s="1">
+        <f>SUM(G42:V42)</f>
+        <v>1410</v>
       </c>
       <c r="G42">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="H42">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="I42">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="J42">
+        <v>81</v>
+      </c>
+      <c r="K42">
+        <v>104</v>
+      </c>
+      <c r="L42">
+        <v>81</v>
+      </c>
+      <c r="M42">
         <v>78</v>
       </c>
-      <c r="K42">
+      <c r="N42">
+        <v>78</v>
+      </c>
+      <c r="O42">
         <v>75</v>
       </c>
-      <c r="L42">
-        <v>87</v>
-      </c>
-      <c r="M42">
-        <v>93</v>
-      </c>
-      <c r="N42">
-        <v>75</v>
-      </c>
-      <c r="O42">
-        <v>72</v>
-      </c>
       <c r="P42">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="Q42">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="R42">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="S42">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="T42">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="U42">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="V42">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="X42" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y42" s="1">
         <v>30</v>
       </c>
       <c r="Z42" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AA42" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB42" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AC42" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AD42" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AE42" s="1">
         <v>30</v>
       </c>
       <c r="AF42" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AG42" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -3190,8 +3354,12 @@
         <v>29.6</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="3"/>
+        <f>STDEV(G43:V43)</f>
         <v>14.764258644894207</v>
+      </c>
+      <c r="F43" s="1">
+        <f>SUM(G43:V43)</f>
+        <v>1410</v>
       </c>
       <c r="G43">
         <v>96</v>
@@ -3272,108 +3440,116 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1">
-        <f>AVERAGE(X44:AG44)</f>
-        <v>29</v>
+        <f t="shared" si="7"/>
+        <v>29.9</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="3"/>
-        <v>16.839932699786342</v>
+        <f t="shared" si="8"/>
+        <v>11.988188631593459</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" ref="F44:F54" si="9">SUM(G44:V44)</f>
+        <v>1410</v>
       </c>
       <c r="G44">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="H44">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="I44">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="J44">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K44">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="L44">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="M44">
+        <v>93</v>
+      </c>
+      <c r="N44">
+        <v>75</v>
+      </c>
+      <c r="O44">
+        <v>72</v>
+      </c>
+      <c r="P44">
+        <v>108</v>
+      </c>
+      <c r="Q44">
+        <v>86</v>
+      </c>
+      <c r="R44">
+        <v>87</v>
+      </c>
+      <c r="S44">
+        <v>102</v>
+      </c>
+      <c r="T44">
+        <v>101</v>
+      </c>
+      <c r="U44">
         <v>78</v>
       </c>
-      <c r="N44">
-        <v>78</v>
-      </c>
-      <c r="O44">
+      <c r="V44">
         <v>75</v>
       </c>
-      <c r="P44">
-        <v>83</v>
-      </c>
-      <c r="Q44">
-        <v>102</v>
-      </c>
-      <c r="R44">
-        <v>84</v>
-      </c>
-      <c r="S44">
-        <v>90</v>
-      </c>
-      <c r="T44">
-        <v>79</v>
-      </c>
-      <c r="U44">
-        <v>68</v>
-      </c>
-      <c r="V44">
-        <v>110</v>
-      </c>
       <c r="X44" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y44" s="1">
         <v>30</v>
       </c>
       <c r="Z44" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA44" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AB44" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC44" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AD44" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE44" s="1">
         <v>30</v>
       </c>
       <c r="AF44" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AG44" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C45" s="1">
-        <f>AVERAGE(X45:AG45)</f>
+        <f t="shared" si="7"/>
         <v>74.400000000000006</v>
       </c>
       <c r="E45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>12.878276282173792</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="9"/>
+        <v>1410</v>
       </c>
       <c r="G45">
         <v>90</v>
@@ -3454,17 +3630,21 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="1">
-        <f>AVERAGE(X46:AG46)</f>
+        <f t="shared" si="7"/>
         <v>40.4</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>11.236102527122116</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="9"/>
+        <v>1410</v>
       </c>
       <c r="G46">
         <v>86</v>
@@ -3545,381 +3725,401 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C47" s="1">
         <f>AVERAGE(X47:AG47)</f>
+        <v>38.6</v>
+      </c>
+      <c r="E47" s="1">
+        <f>STDEV(G47:V47)</f>
+        <v>77.64953316021932</v>
+      </c>
+      <c r="F47" s="1">
+        <f>SUM(G47:V47)</f>
+        <v>1410</v>
+      </c>
+      <c r="G47">
+        <v>87</v>
+      </c>
+      <c r="H47">
+        <v>173</v>
+      </c>
+      <c r="I47">
+        <v>194</v>
+      </c>
+      <c r="J47">
+        <v>168</v>
+      </c>
+      <c r="K47">
+        <v>174</v>
+      </c>
+      <c r="L47">
+        <v>177</v>
+      </c>
+      <c r="M47">
+        <v>135</v>
+      </c>
+      <c r="N47">
+        <v>78</v>
+      </c>
+      <c r="O47">
+        <v>125</v>
+      </c>
+      <c r="P47">
+        <v>99</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>0</v>
+      </c>
+      <c r="X47" s="1">
+        <v>39</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>38</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>37</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>39</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>39</v>
+      </c>
+      <c r="AC47" s="1">
+        <v>40</v>
+      </c>
+      <c r="AD47" s="1">
+        <v>39</v>
+      </c>
+      <c r="AE47" s="1">
+        <v>40</v>
+      </c>
+      <c r="AF47" s="1">
+        <v>38</v>
+      </c>
+      <c r="AG47" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="7"/>
         <v>31.5</v>
       </c>
-      <c r="E47" s="1">
-        <f t="shared" si="3"/>
+      <c r="E48" s="1">
+        <f t="shared" si="8"/>
         <v>10.210288928331069</v>
       </c>
-      <c r="G47">
+      <c r="F48" s="1">
+        <f t="shared" si="9"/>
+        <v>1410</v>
+      </c>
+      <c r="G48">
         <v>99</v>
       </c>
-      <c r="H47">
+      <c r="H48">
         <v>95</v>
       </c>
-      <c r="I47">
+      <c r="I48">
         <v>83</v>
       </c>
-      <c r="J47">
+      <c r="J48">
         <v>80</v>
       </c>
-      <c r="K47">
+      <c r="K48">
         <v>96</v>
       </c>
-      <c r="L47">
+      <c r="L48">
         <v>96</v>
       </c>
-      <c r="M47">
+      <c r="M48">
         <v>86</v>
       </c>
-      <c r="N47">
+      <c r="N48">
         <v>93</v>
       </c>
-      <c r="O47">
+      <c r="O48">
         <v>90</v>
       </c>
-      <c r="P47">
+      <c r="P48">
         <v>72</v>
       </c>
-      <c r="Q47">
+      <c r="Q48">
         <v>108</v>
       </c>
-      <c r="R47">
+      <c r="R48">
         <v>72</v>
       </c>
-      <c r="S47">
+      <c r="S48">
         <v>74</v>
       </c>
-      <c r="T47">
+      <c r="T48">
         <v>84</v>
       </c>
-      <c r="U47">
+      <c r="U48">
         <v>92</v>
       </c>
-      <c r="V47">
+      <c r="V48">
         <v>90</v>
       </c>
-      <c r="X47" s="1">
+      <c r="X48" s="1">
         <v>31</v>
       </c>
-      <c r="Y47" s="1">
+      <c r="Y48" s="1">
         <v>32</v>
       </c>
-      <c r="Z47" s="1">
-        <v>30</v>
-      </c>
-      <c r="AA47" s="1">
+      <c r="Z48" s="1">
+        <v>30</v>
+      </c>
+      <c r="AA48" s="1">
         <v>33</v>
       </c>
-      <c r="AB47" s="1">
+      <c r="AB48" s="1">
         <v>31</v>
       </c>
-      <c r="AC47" s="1">
+      <c r="AC48" s="1">
         <v>33</v>
       </c>
-      <c r="AD47" s="1">
-        <v>30</v>
-      </c>
-      <c r="AE47" s="1">
+      <c r="AD48" s="1">
+        <v>30</v>
+      </c>
+      <c r="AE48" s="1">
         <v>33</v>
       </c>
-      <c r="AF47" s="1">
-        <v>29</v>
-      </c>
-      <c r="AG47" s="1">
+      <c r="AF48" s="1">
+        <v>29</v>
+      </c>
+      <c r="AG48" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="1">
-        <f>AVERAGE(X48:AG48)</f>
-        <v>38.6</v>
-      </c>
-      <c r="E48" s="1">
-        <f t="shared" si="3"/>
-        <v>77.64953316021932</v>
-      </c>
-      <c r="G48">
-        <v>87</v>
-      </c>
-      <c r="H48">
-        <v>173</v>
-      </c>
-      <c r="I48">
-        <v>194</v>
-      </c>
-      <c r="J48">
-        <v>168</v>
-      </c>
-      <c r="K48">
-        <v>174</v>
-      </c>
-      <c r="L48">
-        <v>177</v>
-      </c>
-      <c r="M48">
-        <v>135</v>
-      </c>
-      <c r="N48">
-        <v>78</v>
-      </c>
-      <c r="O48">
-        <v>125</v>
-      </c>
-      <c r="P48">
-        <v>99</v>
-      </c>
-      <c r="Q48">
-        <v>0</v>
-      </c>
-      <c r="R48">
-        <v>0</v>
-      </c>
-      <c r="S48">
-        <v>0</v>
-      </c>
-      <c r="T48">
-        <v>0</v>
-      </c>
-      <c r="U48">
-        <v>0</v>
-      </c>
-      <c r="V48">
-        <v>0</v>
-      </c>
-      <c r="X48" s="1">
-        <v>39</v>
-      </c>
-      <c r="Y48" s="1">
-        <v>38</v>
-      </c>
-      <c r="Z48" s="1">
-        <v>37</v>
-      </c>
-      <c r="AA48" s="1">
-        <v>39</v>
-      </c>
-      <c r="AB48" s="1">
-        <v>39</v>
-      </c>
-      <c r="AC48" s="1">
-        <v>40</v>
-      </c>
-      <c r="AD48" s="1">
-        <v>39</v>
-      </c>
-      <c r="AE48" s="1">
-        <v>40</v>
-      </c>
-      <c r="AF48" s="1">
-        <v>38</v>
-      </c>
-      <c r="AG48" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="1">
         <f>AVERAGE(X49:AG49)</f>
-        <v>31.1</v>
+        <v>31.2</v>
       </c>
       <c r="E49" s="1">
         <f>STDEV(G49:V49)</f>
+        <v>13.652228145373682</v>
+      </c>
+      <c r="F49" s="1">
+        <f>SUM(G49:V49)</f>
+        <v>1410</v>
+      </c>
+      <c r="G49">
+        <v>101</v>
+      </c>
+      <c r="H49">
+        <v>68</v>
+      </c>
+      <c r="I49">
+        <v>93</v>
+      </c>
+      <c r="J49">
+        <v>77</v>
+      </c>
+      <c r="K49">
+        <v>90</v>
+      </c>
+      <c r="L49">
+        <v>99</v>
+      </c>
+      <c r="M49">
+        <v>69</v>
+      </c>
+      <c r="N49">
+        <v>84</v>
+      </c>
+      <c r="O49">
+        <v>84</v>
+      </c>
+      <c r="P49">
+        <v>93</v>
+      </c>
+      <c r="Q49">
+        <v>80</v>
+      </c>
+      <c r="R49">
+        <v>121</v>
+      </c>
+      <c r="S49">
+        <v>99</v>
+      </c>
+      <c r="T49">
+        <v>78</v>
+      </c>
+      <c r="U49">
+        <v>96</v>
+      </c>
+      <c r="V49">
+        <v>78</v>
+      </c>
+      <c r="X49" s="1">
+        <v>29</v>
+      </c>
+      <c r="Y49" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z49" s="1">
+        <v>31</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB49" s="1">
+        <v>29</v>
+      </c>
+      <c r="AC49" s="1">
+        <v>33</v>
+      </c>
+      <c r="AD49" s="1">
+        <v>32</v>
+      </c>
+      <c r="AE49" s="1">
+        <v>35</v>
+      </c>
+      <c r="AF49" s="1">
+        <v>29</v>
+      </c>
+      <c r="AG49" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="7"/>
+        <v>31.1</v>
+      </c>
+      <c r="E50" s="1">
+        <f>STDEV(G50:V50)</f>
         <v>553.3225099343058</v>
       </c>
-      <c r="G49">
+      <c r="F50" s="1">
+        <f t="shared" si="9"/>
+        <v>51044</v>
+      </c>
+      <c r="G50">
         <v>4361</v>
       </c>
-      <c r="H49">
+      <c r="H50">
         <v>3244</v>
       </c>
-      <c r="I49">
+      <c r="I50">
         <v>2985</v>
       </c>
-      <c r="J49">
+      <c r="J50">
         <v>2992</v>
       </c>
-      <c r="K49">
+      <c r="K50">
         <v>2985</v>
       </c>
-      <c r="L49">
+      <c r="L50">
         <v>3450</v>
       </c>
-      <c r="M49">
+      <c r="M50">
         <v>3208</v>
       </c>
-      <c r="N49">
+      <c r="N50">
         <v>4117</v>
       </c>
-      <c r="O49">
+      <c r="O50">
         <v>2560</v>
       </c>
-      <c r="P49">
+      <c r="P50">
         <v>3685</v>
       </c>
-      <c r="Q49">
+      <c r="Q50">
         <v>2897</v>
       </c>
-      <c r="R49">
+      <c r="R50">
         <v>2789</v>
       </c>
-      <c r="S49">
+      <c r="S50">
         <v>3721</v>
       </c>
-      <c r="T49">
+      <c r="T50">
         <v>2782</v>
       </c>
-      <c r="U49">
+      <c r="U50">
         <v>2960</v>
       </c>
-      <c r="V49">
+      <c r="V50">
         <v>2308</v>
       </c>
-      <c r="X49" s="1">
+      <c r="X50" s="1">
         <v>31</v>
       </c>
-      <c r="Y49" s="1">
+      <c r="Y50" s="1">
         <v>32</v>
       </c>
-      <c r="Z49" s="1">
+      <c r="Z50" s="1">
         <v>32</v>
       </c>
-      <c r="AA49" s="1">
-        <v>29</v>
-      </c>
-      <c r="AB49" s="1">
-        <v>30</v>
-      </c>
-      <c r="AC49" s="1">
+      <c r="AA50" s="1">
+        <v>29</v>
+      </c>
+      <c r="AB50" s="1">
+        <v>30</v>
+      </c>
+      <c r="AC50" s="1">
         <v>32</v>
       </c>
-      <c r="AD49" s="1">
+      <c r="AD50" s="1">
         <v>31</v>
       </c>
-      <c r="AE49" s="1">
+      <c r="AE50" s="1">
         <v>31</v>
       </c>
-      <c r="AF49" s="1">
+      <c r="AF50" s="1">
         <v>31</v>
       </c>
-      <c r="AG49" s="1">
+      <c r="AG50" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="1">
-        <f>AVERAGE(X50:AG50)</f>
-        <v>31.2</v>
-      </c>
-      <c r="E50" s="1">
-        <f t="shared" ref="E49:E54" si="4">STDEV(G50:V50)</f>
-        <v>13.652228145373682</v>
-      </c>
-      <c r="G50">
-        <v>101</v>
-      </c>
-      <c r="H50">
-        <v>68</v>
-      </c>
-      <c r="I50">
-        <v>93</v>
-      </c>
-      <c r="J50">
-        <v>77</v>
-      </c>
-      <c r="K50">
-        <v>90</v>
-      </c>
-      <c r="L50">
-        <v>99</v>
-      </c>
-      <c r="M50">
-        <v>69</v>
-      </c>
-      <c r="N50">
-        <v>84</v>
-      </c>
-      <c r="O50">
-        <v>84</v>
-      </c>
-      <c r="P50">
-        <v>93</v>
-      </c>
-      <c r="Q50">
-        <v>80</v>
-      </c>
-      <c r="R50">
-        <v>121</v>
-      </c>
-      <c r="S50">
-        <v>99</v>
-      </c>
-      <c r="T50">
-        <v>78</v>
-      </c>
-      <c r="U50">
-        <v>96</v>
-      </c>
-      <c r="V50">
-        <v>78</v>
-      </c>
-      <c r="X50" s="1">
-        <v>29</v>
-      </c>
-      <c r="Y50" s="1">
-        <v>30</v>
-      </c>
-      <c r="Z50" s="1">
-        <v>31</v>
-      </c>
-      <c r="AA50" s="1">
-        <v>33</v>
-      </c>
-      <c r="AB50" s="1">
-        <v>29</v>
-      </c>
-      <c r="AC50" s="1">
-        <v>33</v>
-      </c>
-      <c r="AD50" s="1">
-        <v>32</v>
-      </c>
-      <c r="AE50" s="1">
-        <v>35</v>
-      </c>
-      <c r="AF50" s="1">
-        <v>29</v>
-      </c>
-      <c r="AG50" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C51">
-        <f>AVERAGE(X51:AG51)</f>
+        <f t="shared" si="7"/>
         <v>30.2</v>
       </c>
       <c r="E51">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E51:E53" si="10">STDEV(G51:V51)</f>
         <v>139.85705500021561</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="9"/>
+        <v>5513</v>
       </c>
       <c r="G51">
         <v>232</v>
@@ -4000,17 +4200,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="1">
-        <f>AVERAGE(X52:AG52)</f>
+        <f t="shared" si="7"/>
         <v>30.1</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>12.622070617242905</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="9"/>
+        <v>1410</v>
       </c>
       <c r="G52">
         <v>75</v>
@@ -4091,17 +4295,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C53" s="1">
-        <f>AVERAGE(X53:AG53)</f>
+        <f t="shared" si="7"/>
         <v>32.6</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>97.605242345548902</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="9"/>
+        <v>1410</v>
       </c>
       <c r="G53">
         <v>413</v>
@@ -4182,18 +4390,22 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="1">
-        <f>AVERAGE(X54:AG54)</f>
+        <f t="shared" si="7"/>
         <v>32.299999999999997</v>
       </c>
       <c r="E54" s="1">
         <f>STDEV(G54:V54)</f>
         <v>352.5</v>
       </c>
+      <c r="F54" s="1">
+        <f t="shared" si="9"/>
+        <v>1410</v>
+      </c>
       <c r="G54">
         <v>1410</v>
       </c>
@@ -4273,28 +4485,34 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="1">
-        <f>AVERAGE(X58:AG58)</f>
+      <c r="C58" s="3">
+        <f t="shared" ref="C58:C70" si="11">AVERAGE(X58:AG58)</f>
         <v>45.1</v>
       </c>
-      <c r="E58" s="1">
-        <f t="shared" ref="E58:E70" si="5">STDEV(G58:V58)</f>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3">
+        <f t="shared" ref="E58:E70" si="12">STDEV(G58:V58)</f>
         <v>20.835766524576595</v>
       </c>
       <c r="G58">
@@ -4376,74 +4594,75 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="1">
+        <v>14</v>
+      </c>
+      <c r="C59" s="3">
         <f>AVERAGE(X59:AG59)</f>
-        <v>45.8</v>
-      </c>
-      <c r="E59" s="1">
-        <f t="shared" si="5"/>
-        <v>29.783384629689085</v>
+        <v>46.3</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3">
+        <f>STDEV(G59:V59)</f>
+        <v>19.76486782146544</v>
       </c>
       <c r="G59">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="H59">
-        <v>436</v>
+        <v>357</v>
       </c>
       <c r="I59">
-        <v>411</v>
+        <v>343</v>
       </c>
       <c r="J59">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="K59">
+        <v>356</v>
+      </c>
+      <c r="L59">
+        <v>352</v>
+      </c>
+      <c r="M59">
+        <v>394</v>
+      </c>
+      <c r="N59">
+        <v>382</v>
+      </c>
+      <c r="O59">
+        <v>373</v>
+      </c>
+      <c r="P59">
+        <v>396</v>
+      </c>
+      <c r="Q59">
+        <v>362</v>
+      </c>
+      <c r="R59">
+        <v>336</v>
+      </c>
+      <c r="S59">
+        <v>362</v>
+      </c>
+      <c r="T59">
+        <v>381</v>
+      </c>
+      <c r="U59">
         <v>384</v>
       </c>
-      <c r="L59">
-        <v>363</v>
-      </c>
-      <c r="M59">
-        <v>350</v>
-      </c>
-      <c r="N59">
-        <v>320</v>
-      </c>
-      <c r="O59">
-        <v>351</v>
-      </c>
-      <c r="P59">
-        <v>334</v>
-      </c>
-      <c r="Q59">
-        <v>341</v>
-      </c>
-      <c r="R59">
-        <v>345</v>
-      </c>
-      <c r="S59">
-        <v>381</v>
-      </c>
-      <c r="T59">
-        <v>361</v>
-      </c>
-      <c r="U59">
-        <v>350</v>
-      </c>
       <c r="V59">
-        <v>381</v>
+        <v>339</v>
       </c>
       <c r="X59" s="1">
+        <v>47</v>
+      </c>
+      <c r="Y59" s="1">
+        <v>45</v>
+      </c>
+      <c r="Z59" s="1">
         <v>46</v>
-      </c>
-      <c r="Y59" s="1">
-        <v>43</v>
-      </c>
-      <c r="Z59" s="1">
-        <v>44</v>
       </c>
       <c r="AA59" s="1">
         <v>46</v>
@@ -4452,31 +4671,32 @@
         <v>44</v>
       </c>
       <c r="AC59" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AD59" s="1">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AE59" s="1">
+        <v>47</v>
+      </c>
+      <c r="AF59" s="1">
+        <v>45</v>
+      </c>
+      <c r="AG59" s="1">
         <v>48</v>
       </c>
-      <c r="AF59" s="1">
-        <v>43</v>
-      </c>
-      <c r="AG59" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="3">
         <f>AVERAGE(X60:AG60)</f>
         <v>45.9</v>
       </c>
-      <c r="E60" s="1">
-        <f t="shared" si="5"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3">
+        <f>STDEV(G60:V60)</f>
         <v>18.0476221887169</v>
       </c>
       <c r="G60">
@@ -4558,74 +4778,75 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C61" s="1">
-        <f>AVERAGE(X61:AG61)</f>
-        <v>46.3</v>
-      </c>
-      <c r="E61" s="1">
-        <f t="shared" si="5"/>
-        <v>19.76486782146544</v>
+        <v>5</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="11"/>
+        <v>45.8</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3">
+        <f t="shared" si="12"/>
+        <v>29.783384629689085</v>
       </c>
       <c r="G61">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="H61">
-        <v>357</v>
+        <v>436</v>
       </c>
       <c r="I61">
-        <v>343</v>
+        <v>411</v>
       </c>
       <c r="J61">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="K61">
-        <v>356</v>
+        <v>384</v>
       </c>
       <c r="L61">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="M61">
-        <v>394</v>
+        <v>350</v>
       </c>
       <c r="N61">
-        <v>382</v>
+        <v>320</v>
       </c>
       <c r="O61">
-        <v>373</v>
+        <v>351</v>
       </c>
       <c r="P61">
-        <v>396</v>
+        <v>334</v>
       </c>
       <c r="Q61">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="R61">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="S61">
-        <v>362</v>
+        <v>381</v>
       </c>
       <c r="T61">
+        <v>361</v>
+      </c>
+      <c r="U61">
+        <v>350</v>
+      </c>
+      <c r="V61">
         <v>381</v>
       </c>
-      <c r="U61">
-        <v>384</v>
-      </c>
-      <c r="V61">
-        <v>339</v>
-      </c>
       <c r="X61" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y61" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Z61" s="1">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AA61" s="1">
         <v>46</v>
@@ -4634,31 +4855,32 @@
         <v>44</v>
       </c>
       <c r="AC61" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AD61" s="1">
+        <v>52</v>
+      </c>
+      <c r="AE61" s="1">
         <v>48</v>
       </c>
-      <c r="AE61" s="1">
-        <v>47</v>
-      </c>
       <c r="AF61" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AG61" s="1">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="1">
-        <f>AVERAGE(X62:AG62)</f>
+      <c r="C62" s="3">
+        <f t="shared" si="11"/>
         <v>166.8</v>
       </c>
-      <c r="E62" s="1">
-        <f t="shared" si="5"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3">
+        <f t="shared" si="12"/>
         <v>17.429859437184227</v>
       </c>
       <c r="G62">
@@ -4740,16 +4962,17 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="1">
-        <f>AVERAGE(X63:AG63)</f>
+      <c r="C63" s="3">
+        <f t="shared" si="11"/>
         <v>78.599999999999994</v>
       </c>
-      <c r="E63" s="1">
-        <f t="shared" si="5"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3">
+        <f t="shared" si="12"/>
         <v>22.404984564452022</v>
       </c>
       <c r="G63">
@@ -4831,380 +5054,385 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="3">
+        <f>AVERAGE(X64:AG64)</f>
+        <v>69</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3">
+        <f>STDEV(G64:V64)</f>
+        <v>330.31681761605779</v>
+      </c>
+      <c r="G64">
+        <v>338</v>
+      </c>
+      <c r="H64">
+        <v>751</v>
+      </c>
+      <c r="I64">
+        <v>697</v>
+      </c>
+      <c r="J64">
+        <v>768</v>
+      </c>
+      <c r="K64">
+        <v>723</v>
+      </c>
+      <c r="L64">
+        <v>705</v>
+      </c>
+      <c r="M64">
+        <v>776</v>
+      </c>
+      <c r="N64">
+        <v>387</v>
+      </c>
+      <c r="O64">
+        <v>323</v>
+      </c>
+      <c r="P64">
+        <v>364</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <v>0</v>
+      </c>
+      <c r="V64">
+        <v>0</v>
+      </c>
+      <c r="X64">
+        <v>66</v>
+      </c>
+      <c r="Y64">
+        <v>66</v>
+      </c>
+      <c r="Z64">
+        <v>78</v>
+      </c>
+      <c r="AA64">
+        <v>72</v>
+      </c>
+      <c r="AB64">
+        <v>72</v>
+      </c>
+      <c r="AC64">
+        <v>72</v>
+      </c>
+      <c r="AD64">
+        <v>66</v>
+      </c>
+      <c r="AE64">
+        <v>66</v>
+      </c>
+      <c r="AF64">
+        <v>66</v>
+      </c>
+      <c r="AG64">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="1">
-        <f>AVERAGE(X64:AG64)</f>
+      <c r="C65" s="3">
+        <f t="shared" si="11"/>
         <v>51.6</v>
       </c>
-      <c r="E64" s="1">
-        <f t="shared" si="5"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3">
+        <f t="shared" si="12"/>
         <v>24.868236098820251</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <v>408</v>
       </c>
-      <c r="H64">
+      <c r="H65">
         <v>360</v>
       </c>
-      <c r="I64">
+      <c r="I65">
         <v>348</v>
       </c>
-      <c r="J64">
+      <c r="J65">
         <v>360</v>
       </c>
-      <c r="K64">
+      <c r="K65">
         <v>350</v>
       </c>
-      <c r="L64">
+      <c r="L65">
         <v>374</v>
       </c>
-      <c r="M64">
+      <c r="M65">
         <v>362</v>
       </c>
-      <c r="N64">
+      <c r="N65">
         <v>341</v>
       </c>
-      <c r="O64">
+      <c r="O65">
         <v>349</v>
       </c>
-      <c r="P64">
+      <c r="P65">
         <v>407</v>
       </c>
-      <c r="Q64">
+      <c r="Q65">
         <v>370</v>
       </c>
-      <c r="R64">
+      <c r="R65">
         <v>328</v>
       </c>
-      <c r="S64">
+      <c r="S65">
         <v>367</v>
       </c>
-      <c r="T64">
+      <c r="T65">
         <v>381</v>
       </c>
-      <c r="U64">
+      <c r="U65">
         <v>415</v>
       </c>
-      <c r="V64">
+      <c r="V65">
         <v>355</v>
       </c>
-      <c r="X64" s="1">
+      <c r="X65" s="1">
         <v>51</v>
       </c>
-      <c r="Y64" s="1">
+      <c r="Y65" s="1">
         <v>51</v>
       </c>
-      <c r="Z64" s="1">
+      <c r="Z65" s="1">
         <v>50</v>
       </c>
-      <c r="AA64" s="1">
+      <c r="AA65" s="1">
         <v>50</v>
       </c>
-      <c r="AB64" s="1">
+      <c r="AB65" s="1">
         <v>52</v>
       </c>
-      <c r="AC64" s="1">
+      <c r="AC65" s="1">
         <v>51</v>
       </c>
-      <c r="AD64" s="1">
+      <c r="AD65" s="1">
         <v>52</v>
       </c>
-      <c r="AE64" s="1">
+      <c r="AE65" s="1">
         <v>52</v>
       </c>
-      <c r="AF64" s="1">
+      <c r="AF65" s="1">
         <v>53</v>
       </c>
-      <c r="AG64" s="1">
+      <c r="AG65" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" s="1">
-        <f>AVERAGE(X65:AG65)</f>
-        <v>69</v>
-      </c>
-      <c r="E65" s="1">
-        <f t="shared" si="5"/>
-        <v>330.31681761605779</v>
-      </c>
-      <c r="G65">
-        <v>338</v>
-      </c>
-      <c r="H65">
-        <v>751</v>
-      </c>
-      <c r="I65">
-        <v>697</v>
-      </c>
-      <c r="J65">
-        <v>768</v>
-      </c>
-      <c r="K65">
-        <v>723</v>
-      </c>
-      <c r="L65">
-        <v>705</v>
-      </c>
-      <c r="M65">
-        <v>776</v>
-      </c>
-      <c r="N65">
-        <v>387</v>
-      </c>
-      <c r="O65">
-        <v>323</v>
-      </c>
-      <c r="P65">
-        <v>364</v>
-      </c>
-      <c r="Q65">
-        <v>0</v>
-      </c>
-      <c r="R65">
-        <v>0</v>
-      </c>
-      <c r="S65">
-        <v>0</v>
-      </c>
-      <c r="T65">
-        <v>0</v>
-      </c>
-      <c r="U65">
-        <v>0</v>
-      </c>
-      <c r="V65">
-        <v>0</v>
-      </c>
-      <c r="X65">
-        <v>66</v>
-      </c>
-      <c r="Y65">
-        <v>66</v>
-      </c>
-      <c r="Z65">
-        <v>78</v>
-      </c>
-      <c r="AA65">
-        <v>72</v>
-      </c>
-      <c r="AB65">
-        <v>72</v>
-      </c>
-      <c r="AC65">
-        <v>72</v>
-      </c>
-      <c r="AD65">
-        <v>66</v>
-      </c>
-      <c r="AE65">
-        <v>66</v>
-      </c>
-      <c r="AF65">
-        <v>66</v>
-      </c>
-      <c r="AG65">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="1">
+        <v>3</v>
+      </c>
+      <c r="C66" s="3">
         <f>AVERAGE(X66:AG66)</f>
-        <v>48.6</v>
-      </c>
-      <c r="E66" s="1">
-        <f t="shared" si="5"/>
-        <v>33.534497163368947</v>
+        <v>50.8</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3">
+        <f>STDEV(G66:V66)</f>
+        <v>13.953344879753146</v>
       </c>
       <c r="G66">
-        <v>364</v>
+        <v>397</v>
       </c>
       <c r="H66">
-        <v>414</v>
+        <v>362</v>
       </c>
       <c r="I66">
-        <v>428</v>
+        <v>369</v>
       </c>
       <c r="J66">
-        <v>392</v>
+        <v>359</v>
       </c>
       <c r="K66">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="L66">
         <v>389</v>
       </c>
       <c r="M66">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="N66">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="O66">
+        <v>361</v>
+      </c>
+      <c r="P66">
+        <v>353</v>
+      </c>
+      <c r="Q66">
+        <v>357</v>
+      </c>
+      <c r="R66">
+        <v>369</v>
+      </c>
+      <c r="S66">
+        <v>375</v>
+      </c>
+      <c r="T66">
         <v>350</v>
       </c>
-      <c r="P66">
-        <v>331</v>
-      </c>
-      <c r="Q66">
-        <v>300</v>
-      </c>
-      <c r="R66">
-        <v>338</v>
-      </c>
-      <c r="S66">
-        <v>337</v>
-      </c>
-      <c r="T66">
-        <v>359</v>
-      </c>
       <c r="U66">
-        <v>392</v>
+        <v>355</v>
       </c>
       <c r="V66">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="X66" s="1">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="Y66" s="1">
+        <v>51</v>
+      </c>
+      <c r="Z66" s="1">
+        <v>52</v>
+      </c>
+      <c r="AA66" s="1">
+        <v>52</v>
+      </c>
+      <c r="AB66" s="1">
         <v>50</v>
-      </c>
-      <c r="Z66" s="1">
-        <v>48</v>
-      </c>
-      <c r="AA66" s="1">
-        <v>47</v>
-      </c>
-      <c r="AB66" s="1">
-        <v>49</v>
       </c>
       <c r="AC66" s="1">
         <v>50</v>
       </c>
       <c r="AD66" s="1">
+        <v>51</v>
+      </c>
+      <c r="AE66" s="1">
         <v>48</v>
       </c>
-      <c r="AE66" s="1">
+      <c r="AF66" s="1">
+        <v>53</v>
+      </c>
+      <c r="AG66" s="1">
         <v>50</v>
       </c>
-      <c r="AF66" s="1">
-        <v>47</v>
-      </c>
-      <c r="AG66" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" s="1">
-        <f>AVERAGE(X67:AG67)</f>
-        <v>50.8</v>
-      </c>
-      <c r="E67" s="1">
-        <f t="shared" si="5"/>
-        <v>13.953344879753146</v>
+        <v>4</v>
+      </c>
+      <c r="C67" s="3">
+        <f t="shared" si="11"/>
+        <v>48.6</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3">
+        <f t="shared" si="12"/>
+        <v>33.534497163368947</v>
       </c>
       <c r="G67">
-        <v>397</v>
+        <v>364</v>
       </c>
       <c r="H67">
-        <v>362</v>
+        <v>414</v>
       </c>
       <c r="I67">
+        <v>428</v>
+      </c>
+      <c r="J67">
+        <v>392</v>
+      </c>
+      <c r="K67">
         <v>369</v>
-      </c>
-      <c r="J67">
-        <v>359</v>
-      </c>
-      <c r="K67">
-        <v>376</v>
       </c>
       <c r="L67">
         <v>389</v>
       </c>
       <c r="M67">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="N67">
-        <v>362</v>
+        <v>378</v>
       </c>
       <c r="O67">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="P67">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="Q67">
-        <v>357</v>
+        <v>300</v>
       </c>
       <c r="R67">
-        <v>369</v>
+        <v>338</v>
       </c>
       <c r="S67">
-        <v>375</v>
+        <v>337</v>
       </c>
       <c r="T67">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="U67">
-        <v>355</v>
+        <v>392</v>
       </c>
       <c r="V67">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="X67" s="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Y67" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z67" s="1">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AA67" s="1">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="AB67" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AC67" s="1">
         <v>50</v>
       </c>
       <c r="AD67" s="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AE67" s="1">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AF67" s="1">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="AG67" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="1">
-        <f>AVERAGE(X68:AG68)</f>
+      <c r="C68" s="3">
+        <f t="shared" si="11"/>
         <v>47.7</v>
       </c>
-      <c r="E68" s="1">
-        <f t="shared" si="5"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3">
+        <f t="shared" si="12"/>
         <v>33.534497163368947</v>
       </c>
       <c r="G68">
@@ -5286,16 +5514,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="1">
-        <f>AVERAGE(X69:AG69)</f>
+      <c r="C69" s="3">
+        <f t="shared" si="11"/>
         <v>93.6</v>
       </c>
-      <c r="E69" s="1">
-        <f t="shared" si="5"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3">
+        <f t="shared" si="12"/>
         <v>51.680912014656499</v>
       </c>
       <c r="G69">
@@ -5377,16 +5606,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C70" s="1">
-        <f>AVERAGE(X70:AG70)</f>
+      <c r="C70" s="3">
+        <f t="shared" si="11"/>
         <v>54.5</v>
       </c>
-      <c r="E70" s="1">
-        <f t="shared" si="5"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3">
+        <f t="shared" si="12"/>
         <v>458.7906521497577</v>
       </c>
       <c r="G70">
@@ -5468,124 +5698,59 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B74">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B76">
-        <v>1993</v>
-      </c>
-    </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77">
-        <v>2185</v>
-      </c>
-    </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B79">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B80">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B81">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B84">
-        <v>2771</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B85">
-        <v>3551</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B87" t="s">
-        <v>24</v>
-      </c>
+      <c r="C71" s="3">
+        <v>0</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>